<commit_message>
Add expected error code to test-challenges
</commit_message>
<xml_diff>
--- a/spec/fixtures/test-data/test-challenges.xlsx
+++ b/spec/fixtures/test-data/test-challenges.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12580" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="102">
   <si>
     <t>A14</t>
   </si>
@@ -658,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,10 +669,11 @@
     <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -682,8 +683,11 @@
       <c r="C1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="D1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -693,8 +697,11 @@
       <c r="C2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -704,8 +711,11 @@
       <c r="C3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -715,8 +725,11 @@
       <c r="C4" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -726,11 +739,14 @@
       <c r="C5" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -740,8 +756,11 @@
       <c r="C6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -751,8 +770,11 @@
       <c r="C7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -762,8 +784,11 @@
       <c r="C8" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -773,11 +798,14 @@
       <c r="C9" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -787,11 +815,14 @@
       <c r="C10" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -801,8 +832,11 @@
       <c r="C11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -812,8 +846,11 @@
       <c r="C12" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -823,8 +860,11 @@
       <c r="C13" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -834,8 +874,11 @@
       <c r="C14" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -845,11 +888,14 @@
       <c r="C15" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -859,8 +905,11 @@
       <c r="C16" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -870,8 +919,11 @@
       <c r="C17" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -881,8 +933,11 @@
       <c r="C18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -892,8 +947,11 @@
       <c r="C19" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -903,8 +961,11 @@
       <c r="C20" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -914,8 +975,11 @@
       <c r="C21" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -925,11 +989,14 @@
       <c r="C22" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -939,8 +1006,11 @@
       <c r="C23" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -950,8 +1020,11 @@
       <c r="C24" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -961,8 +1034,11 @@
       <c r="C25" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -972,8 +1048,11 @@
       <c r="C26" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -983,8 +1062,11 @@
       <c r="C27" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -994,8 +1076,11 @@
       <c r="C28" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -1005,8 +1090,11 @@
       <c r="C29" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1016,8 +1104,11 @@
       <c r="C30" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -1027,8 +1118,11 @@
       <c r="C31" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1038,8 +1132,11 @@
       <c r="C32" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1049,11 +1146,14 @@
       <c r="C33" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>94</v>
       </c>
@@ -1063,8 +1163,11 @@
       <c r="C34" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>72</v>
       </c>
@@ -1073,6 +1176,23 @@
       </c>
       <c r="C35" t="s">
         <v>100</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>72</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update correct error codes in test-challenges
</commit_message>
<xml_diff>
--- a/spec/fixtures/test-data/test-challenges.xlsx
+++ b/spec/fixtures/test-data/test-challenges.xlsx
@@ -661,7 +661,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -990,7 +990,7 @@
         <v>86</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>87</v>
@@ -1147,7 +1147,7 @@
         <v>66</v>
       </c>
       <c r="D33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>87</v>
@@ -1192,7 +1192,7 @@
         <v>100</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mock data for final spots after switches
</commit_message>
<xml_diff>
--- a/spec/fixtures/test-data/test-challenges.xlsx
+++ b/spec/fixtures/test-data/test-challenges.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12880" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="28800" yWindow="-4600" windowWidth="20240" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,7 +363,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,7 +664,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>